<commit_message>
Updates to AVMC for freight BEV HDVs reflecting newer data and need to replace battery every 7 years
</commit_message>
<xml_diff>
--- a/InputData/trans/AVMC/Annual Vehicle Maint Cost.xlsx
+++ b/InputData/trans/AVMC/Annual Vehicle Maint Cost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\trans\AVMC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us-analysis\InputData\trans\AVMC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF646FD-413E-4B0A-A984-B8BBA1CEB9B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B3C505-ECAA-49CA-9672-DF5CF56F78F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="405" windowWidth="24435" windowHeight="16275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="140">
   <si>
     <t>Sources:</t>
   </si>
@@ -443,6 +443,27 @@
   </si>
   <si>
     <t>AVMC Annual Vehicle Maintenance Cost</t>
+  </si>
+  <si>
+    <t>2020 USD/yr</t>
+  </si>
+  <si>
+    <t>Freight BEV HDVs</t>
+  </si>
+  <si>
+    <t>LBNL</t>
+  </si>
+  <si>
+    <t>Why Regional and Long-Haul Trucks are Primed for Electrification Now</t>
+  </si>
+  <si>
+    <t>https://eta-publications.lbl.gov/sites/default/files/updated_5_final_ehdv_report_033121.pdf</t>
+  </si>
+  <si>
+    <t>Table 3</t>
+  </si>
+  <si>
+    <t>LBNL: Includes annual ongoing mainteance and annualized battery replacement every 7 years over a 28 year life</t>
   </si>
 </sst>
 </file>
@@ -1868,9 +1889,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B72"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1947,256 +1970,286 @@
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="2" t="s">
-        <v>60</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>61</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="3">
-        <v>2016</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>66</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="9" t="s">
-        <v>67</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" s="3">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" s="9" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="3">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="3">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="9" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2">
-      <c r="B37" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2">
-      <c r="B39" s="3">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2">
-      <c r="B40" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2">
-      <c r="B41" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2">
-      <c r="B42" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" s="3">
-        <v>2013</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48" s="9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51" s="2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53" s="3">
-        <v>2012</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="54" spans="2:2">
       <c r="B54" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="2:2">
       <c r="B55" s="9" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="2:2">
       <c r="B56" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="2:2">
       <c r="B58" s="2" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="2:2">
       <c r="B59" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" spans="2:2">
       <c r="B60" s="3">
-        <v>2018</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="2:2">
       <c r="B62" s="9" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="2:2">
       <c r="B63" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="B65" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="B66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="B67" s="3">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="B68" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="B69" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="B70" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="1" t="s">
+    <row r="72" spans="1:2">
+      <c r="A72" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="1" t="s">
+    <row r="74" spans="1:2">
+      <c r="A74" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
-      <c r="A68">
+    <row r="75" spans="1:2">
+      <c r="A75">
         <v>1.2969999999999999</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B75" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
-      <c r="A69">
+    <row r="76" spans="1:2">
+      <c r="A76">
         <v>0.9143273584567535</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B76" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
-      <c r="A70">
+    <row r="77" spans="1:2">
+      <c r="A77">
         <v>0.95661376543184151</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B77" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
-      <c r="A71">
+    <row r="78" spans="1:2">
+      <c r="A78">
         <v>0.93665959530026111</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B78" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
-      <c r="A72">
+    <row r="79" spans="1:2">
+      <c r="A79">
         <v>1.0663762232760343</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B79" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2204,13 +2257,13 @@
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{F7E7A3DE-93B2-4E97-8034-BE9FA2CBB032}"/>
     <hyperlink ref="B14" r:id="rId2" xr:uid="{0A5F8456-85E2-4B46-98CB-42301965587F}"/>
-    <hyperlink ref="B28" r:id="rId3" display="https://www.icao.int/MID/Documents/2017/Aviation Data and Analysis Seminar/PPT3 - Airlines Operating costs and productivity.pdf" xr:uid="{32C07062-31D6-4D64-9941-54355C398A54}"/>
-    <hyperlink ref="B21" r:id="rId4" xr:uid="{A1682FDD-C2BD-495E-8A6B-5F03193720A5}"/>
-    <hyperlink ref="B35" r:id="rId5" xr:uid="{86CB5594-D53D-4996-A0D1-BB39C7D7D625}"/>
-    <hyperlink ref="B41" r:id="rId6" xr:uid="{B0ED8C7C-30CE-4966-BD3F-14CBF2AB2A2B}"/>
-    <hyperlink ref="B48" r:id="rId7" xr:uid="{B27ABC8E-899E-48AC-8608-F37B2EDFED93}"/>
-    <hyperlink ref="B55" r:id="rId8" display="http://www.sparusa.com/Presentations/Presentation-Commercial Ship Life Cycle &amp; Required Freight Rate (RFR) Cost Model.pdf" xr:uid="{4BC70352-C238-4681-9474-B434C82A9EE6}"/>
-    <hyperlink ref="B62" r:id="rId9" xr:uid="{5439DEF3-45BA-42A3-B033-B27D7C2B3817}"/>
+    <hyperlink ref="B35" r:id="rId3" display="https://www.icao.int/MID/Documents/2017/Aviation Data and Analysis Seminar/PPT3 - Airlines Operating costs and productivity.pdf" xr:uid="{32C07062-31D6-4D64-9941-54355C398A54}"/>
+    <hyperlink ref="B28" r:id="rId4" xr:uid="{A1682FDD-C2BD-495E-8A6B-5F03193720A5}"/>
+    <hyperlink ref="B42" r:id="rId5" xr:uid="{86CB5594-D53D-4996-A0D1-BB39C7D7D625}"/>
+    <hyperlink ref="B48" r:id="rId6" xr:uid="{B0ED8C7C-30CE-4966-BD3F-14CBF2AB2A2B}"/>
+    <hyperlink ref="B55" r:id="rId7" xr:uid="{B27ABC8E-899E-48AC-8608-F37B2EDFED93}"/>
+    <hyperlink ref="B62" r:id="rId8" display="http://www.sparusa.com/Presentations/Presentation-Commercial Ship Life Cycle &amp; Required Freight Rate (RFR) Cost Model.pdf" xr:uid="{4BC70352-C238-4681-9474-B434C82A9EE6}"/>
+    <hyperlink ref="B69" r:id="rId9" xr:uid="{5439DEF3-45BA-42A3-B033-B27D7C2B3817}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
@@ -2219,9 +2272,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA56E7A-E0B4-48E9-AA66-C39B91D43ABA}">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2343,7 +2398,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="12">
-        <f>B18/About!$A$68*About!$A$69</f>
+        <f>B18/About!$A$75*About!$A$76</f>
         <v>656.31362430473212</v>
       </c>
       <c r="C20" t="s">
@@ -2355,7 +2410,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="12">
-        <f>B19/About!$A$68*About!$A$69</f>
+        <f>B19/About!$A$75*About!$A$76</f>
         <v>344.72326776048766</v>
       </c>
       <c r="C21" t="s">
@@ -2383,33 +2438,34 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="2" t="s">
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="10">
+        <f>6500+100*1062*3/28</f>
+        <v>17878.571428571428</v>
+      </c>
+      <c r="C25" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="13">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="C27" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" t="s">
-        <v>48</v>
-      </c>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="B28" s="13">
-        <v>0.22</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C28" t="s">
         <v>47</v>
@@ -2420,37 +2476,39 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29">
-        <v>9270</v>
+        <v>22</v>
+      </c>
+      <c r="B29" s="13">
+        <v>0.22</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="D29" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="13">
-        <f>$B$29*B27</f>
-        <v>2595.6000000000004</v>
+        <v>49</v>
+      </c>
+      <c r="B30">
+        <v>9270</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="B31" s="13">
-        <f>$B$29*B28</f>
-        <v>2039.4</v>
+        <f>$B$30*B28</f>
+        <v>2595.6000000000004</v>
       </c>
       <c r="C31" t="s">
         <v>52</v>
@@ -2458,131 +2516,129 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="B32" s="13">
-        <f>B30*About!$A$70</f>
-        <v>2482.986689554888</v>
+        <f>$B$30*B29</f>
+        <v>2039.4</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="B33" s="13">
-        <f>B31*About!$A$70</f>
-        <v>1950.9181132216977</v>
+        <f>B31*About!$A$77</f>
+        <v>2482.986689554888</v>
       </c>
       <c r="C33" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="B34" s="13"/>
+      <c r="A34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="13">
+        <f>B32*About!$A$77</f>
+        <v>1950.9181132216977</v>
+      </c>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="2" t="s">
+      <c r="B35" s="13"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="11"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
+      <c r="B36" s="18"/>
+      <c r="C36" s="11"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="17">
+      <c r="B37" s="17">
         <v>590</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>71</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="B37" s="17">
-        <f>B36*About!$A$71</f>
+    <row r="38" spans="1:4">
+      <c r="B38" s="17">
+        <f>B37*About!$A$78</f>
         <v>552.6291612271541</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="B38" s="19">
-        <v>11.3</v>
-      </c>
-      <c r="C38" t="s">
-        <v>57</v>
-      </c>
-      <c r="D38" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="B39" s="19">
+        <v>11.3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="B40" s="19">
         <v>365</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="B40" s="17">
-        <f>B37*B38*B39</f>
+    <row r="41" spans="1:4">
+      <c r="B41" s="17">
+        <f>B38*B39*B40</f>
         <v>2279318.9754813975</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="B41" s="17"/>
-    </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="2" t="s">
+      <c r="B42" s="17"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="22"/>
-      <c r="C42" s="11"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" t="s">
+      <c r="B43" s="22"/>
+      <c r="C43" s="11"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
         <v>96</v>
       </c>
-      <c r="B43" s="17"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="23" t="s">
+      <c r="B44" s="17"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="B44" s="17"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
-        <v>84</v>
-      </c>
-      <c r="B45" s="13">
-        <v>14.36</v>
-      </c>
-      <c r="C45" t="s">
-        <v>86</v>
-      </c>
-      <c r="D45" t="s">
-        <v>97</v>
-      </c>
+      <c r="B45" s="17"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B46" s="13">
-        <v>10.49</v>
+        <v>14.36</v>
       </c>
       <c r="C46" t="s">
         <v>86</v>
@@ -2592,429 +2648,443 @@
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="B47" s="17"/>
+      <c r="A47" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="13">
+        <v>10.49</v>
+      </c>
+      <c r="C47" t="s">
+        <v>86</v>
+      </c>
+      <c r="D47" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" t="s">
+      <c r="B48" s="17"/>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
         <v>108</v>
       </c>
-      <c r="B48" s="24">
+      <c r="B49" s="24">
         <f>AVERAGE(21.4,22.7,23.1,25.8,31.2)</f>
         <v>24.839999999999996</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>87</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
         <v>88</v>
       </c>
-      <c r="B49" s="19">
+      <c r="B50" s="19">
         <f>24*365</f>
         <v>8760</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
         <v>89</v>
       </c>
-      <c r="B50" s="5">
-        <f>B48*B49</f>
+      <c r="B51" s="5">
+        <f>B49*B50</f>
         <v>217598.39999999997</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="B51" s="17"/>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
+    <row r="52" spans="1:4">
+      <c r="B52" s="17"/>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
         <v>91</v>
       </c>
-      <c r="B52" s="17">
-        <f>B45*B50</f>
+      <c r="B53" s="17">
+        <f>B46*B51</f>
         <v>3124713.0239999993</v>
-      </c>
-      <c r="C52" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
-        <v>95</v>
-      </c>
-      <c r="B53" s="17">
-        <f>B46*B50</f>
-        <v>2282607.2159999995</v>
       </c>
       <c r="C53" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
+        <v>95</v>
+      </c>
+      <c r="B54" s="17">
+        <f>B47*B51</f>
+        <v>2282607.2159999995</v>
+      </c>
+      <c r="C54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
         <v>91</v>
       </c>
-      <c r="B54" s="17">
-        <f>B52*About!$A$72</f>
+      <c r="B55" s="17">
+        <f>B53*About!$A$79</f>
         <v>3332119.6733545554</v>
-      </c>
-      <c r="C54" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>95</v>
-      </c>
-      <c r="B55" s="17">
-        <f>B53*About!$A$72</f>
-        <v>2434118.0622207024</v>
       </c>
       <c r="C55" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="B56" s="17"/>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="B57" s="13"/>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="2" t="s">
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>95</v>
+      </c>
+      <c r="B56" s="17">
+        <f>B54*About!$A$79</f>
+        <v>2434118.0622207024</v>
+      </c>
+      <c r="C56" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="B57" s="17"/>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="B58" s="13"/>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="18"/>
-      <c r="C58" s="11"/>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" t="s">
+      <c r="B59" s="18"/>
+      <c r="C59" s="11"/>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="17">
+      <c r="B60" s="17">
         <v>1000</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
-      <c r="B60" s="17">
-        <f>B59*About!A69</f>
+    <row r="61" spans="1:4">
+      <c r="B61" s="17">
+        <f>B60*About!A76</f>
         <v>914.32735845675347</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
         <v>75</v>
       </c>
-      <c r="B61" s="13"/>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
+      <c r="B62" s="13"/>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
         <v>76</v>
       </c>
-      <c r="B62" s="13"/>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
+      <c r="B63" s="13"/>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
         <v>77</v>
       </c>
-      <c r="B63" s="13"/>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
+      <c r="B64" s="13"/>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
         <v>78</v>
       </c>
-      <c r="B64" s="13"/>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="9" t="s">
+      <c r="B65" s="13"/>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B65" s="13"/>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" t="s">
+      <c r="B66" s="13"/>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
         <v>80</v>
       </c>
-      <c r="B66" s="13"/>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="2" t="s">
+      <c r="B67" s="13"/>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B68" s="11"/>
-      <c r="C68" s="11"/>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="1" t="s">
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
-      <c r="A70" t="s">
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
         <v>111</v>
       </c>
-      <c r="B70" s="17">
+      <c r="B71" s="17">
         <v>1695890</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C71" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:4">
+      <c r="A73" s="1" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="14" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="14" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
-      <c r="A76" t="s">
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
         <v>111</v>
       </c>
-      <c r="B76" s="25">
+      <c r="B77" s="25">
         <v>0.1</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C77" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="14" t="s">
+    <row r="78" spans="1:4">
+      <c r="A78" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B77" s="10">
+      <c r="B78" s="10">
         <v>30000</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" t="s">
         <v>123</v>
       </c>
-      <c r="D77" s="14" t="s">
+      <c r="D78" s="14" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
-      <c r="A78" t="s">
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
         <v>111</v>
       </c>
-      <c r="B78" s="10">
-        <f>B76*B77</f>
+      <c r="B79" s="10">
+        <f>B77*B78</f>
         <v>3000</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C79" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="15" t="s">
+    <row r="84" spans="1:3">
+      <c r="A84" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B83" s="16"/>
-      <c r="C83" s="16"/>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="16"/>
+      <c r="C84" s="16"/>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="B85" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C85" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="1" t="s">
+    <row r="86" spans="1:3">
+      <c r="A86" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B85" s="20">
+      <c r="B86" s="20">
         <f>B20</f>
         <v>656.31362430473212</v>
       </c>
-      <c r="C85" s="20">
+      <c r="C86" s="20">
         <f>B21</f>
         <v>344.72326776048766</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B86" s="20">
-        <f>B32</f>
-        <v>2482.986689554888</v>
-      </c>
-      <c r="C86" s="20">
-        <f>B33</f>
-        <v>1950.9181132216977</v>
-      </c>
-    </row>
     <row r="87" spans="1:3">
       <c r="A87" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" s="20">
+        <f>B33</f>
+        <v>2482.986689554888</v>
+      </c>
+      <c r="C87" s="20">
+        <f>B34</f>
+        <v>1950.9181132216977</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B87" s="20">
-        <f>B40</f>
+      <c r="B88" s="20">
+        <f>B41</f>
         <v>2279318.9754813975</v>
       </c>
-      <c r="C87" t="e">
+      <c r="C88" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B88" s="20">
-        <f>B54</f>
-        <v>3332119.6733545554</v>
-      </c>
-      <c r="C88" s="20">
-        <f>B55</f>
-        <v>2434118.0622207024</v>
-      </c>
-    </row>
     <row r="89" spans="1:3">
       <c r="A89" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89" s="20">
+        <f>B55</f>
+        <v>3332119.6733545554</v>
+      </c>
+      <c r="C89" s="20">
+        <f>B56</f>
+        <v>2434118.0622207024</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B89" s="20">
-        <f>B78</f>
+      <c r="B90" s="20">
+        <f>B79</f>
         <v>3000</v>
       </c>
-      <c r="C89" t="e">
+      <c r="C90" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="1" t="s">
+    <row r="91" spans="1:3">
+      <c r="A91" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="20">
-        <f>B60</f>
+      <c r="B91" s="20">
+        <f>B61</f>
         <v>914.32735845675347</v>
       </c>
-      <c r="C90" s="21">
-        <f>B90*(C85/B85)</f>
+      <c r="C91" s="21">
+        <f>B91*(C86/B86)</f>
         <v>480.24283381885334</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
-      <c r="A92" s="15" t="s">
+    <row r="93" spans="1:3">
+      <c r="A93" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B92" s="16"/>
-      <c r="C92" s="16"/>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="B93" s="1" t="s">
+      <c r="B93" s="16"/>
+      <c r="C93" s="16"/>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="B94" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C94" s="1" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B94" s="20">
-        <f>B85</f>
-        <v>656.31362430473212</v>
-      </c>
-      <c r="C94" s="20">
-        <f>C85</f>
-        <v>344.72326776048766</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B95" s="20">
+        <f>B86</f>
+        <v>656.31362430473212</v>
+      </c>
+      <c r="C95" s="20">
+        <f>C86</f>
+        <v>344.72326776048766</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B95" s="20">
+      <c r="B96" s="20">
         <f>B24</f>
         <v>15000</v>
       </c>
-      <c r="C95" s="21">
-        <f>B95*(C86/B86)</f>
+      <c r="C96" s="21">
+        <f>B96*(C87/B87)</f>
         <v>11785.714285714286</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
-      <c r="A96" s="1" t="s">
+    <row r="97" spans="1:3">
+      <c r="A97" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B96" s="20">
-        <f>B87</f>
+      <c r="B97" s="20">
+        <f>B88</f>
         <v>2279318.9754813975</v>
       </c>
-      <c r="C96" t="e">
+      <c r="C97" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
-      <c r="A97" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B97" s="20">
-        <f>B54</f>
-        <v>3332119.6733545554</v>
-      </c>
-      <c r="C97" s="20">
-        <f>B55</f>
-        <v>2434118.0622207024</v>
-      </c>
-    </row>
     <row r="98" spans="1:3">
       <c r="A98" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B98" s="20">
+        <f>B55</f>
+        <v>3332119.6733545554</v>
+      </c>
+      <c r="C98" s="20">
+        <f>B56</f>
+        <v>2434118.0622207024</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B98" s="20">
-        <f>B70</f>
+      <c r="B99" s="20">
+        <f>B71</f>
         <v>1695890</v>
       </c>
-      <c r="C98" t="e">
+      <c r="C99" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
-      <c r="A99" s="1" t="s">
+    <row r="100" spans="1:3">
+      <c r="A100" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B99" t="e">
+      <c r="B100" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="C99" t="e">
+      <c r="C100" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
@@ -3023,7 +3093,7 @@
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{DEA7D659-12AB-4A56-889B-D770D6477AD9}"/>
     <hyperlink ref="B13" r:id="rId2" xr:uid="{83856772-5164-484D-9C39-5E905DAB68CE}"/>
-    <hyperlink ref="A65" r:id="rId3" xr:uid="{CF3217FC-13DF-41C0-A64F-4474765B54A2}"/>
+    <hyperlink ref="A66" r:id="rId3" xr:uid="{CF3217FC-13DF-41C0-A64F-4474765B54A2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -3080,31 +3150,31 @@
         <v>2</v>
       </c>
       <c r="B2" s="5">
-        <f>'Cost Data'!$C85</f>
+        <f>'Cost Data'!$C86</f>
         <v>344.72326776048766</v>
       </c>
       <c r="C2" s="5">
-        <f>'Cost Data'!$B85</f>
+        <f>'Cost Data'!$B86</f>
         <v>656.31362430473212</v>
       </c>
       <c r="D2" s="5">
-        <f>'Cost Data'!$B85</f>
+        <f>'Cost Data'!$B86</f>
         <v>656.31362430473212</v>
       </c>
       <c r="E2" s="5">
-        <f>'Cost Data'!$B85</f>
+        <f>'Cost Data'!$B86</f>
         <v>656.31362430473212</v>
       </c>
       <c r="F2" s="5">
-        <f>'Cost Data'!$B85</f>
+        <f>'Cost Data'!$B86</f>
         <v>656.31362430473212</v>
       </c>
       <c r="G2" s="5">
-        <f>'Cost Data'!$B85</f>
+        <f>'Cost Data'!$B86</f>
         <v>656.31362430473212</v>
       </c>
       <c r="H2" s="5">
-        <f>'Cost Data'!$C85</f>
+        <f>'Cost Data'!$C86</f>
         <v>344.72326776048766</v>
       </c>
     </row>
@@ -3113,31 +3183,31 @@
         <v>3</v>
       </c>
       <c r="B3" s="5">
-        <f>'Cost Data'!$C86</f>
+        <f>'Cost Data'!$C87</f>
         <v>1950.9181132216977</v>
       </c>
       <c r="C3" s="5">
-        <f>'Cost Data'!$B86</f>
+        <f>'Cost Data'!$B87</f>
         <v>2482.986689554888</v>
       </c>
       <c r="D3" s="5">
-        <f>'Cost Data'!$B86</f>
+        <f>'Cost Data'!$B87</f>
         <v>2482.986689554888</v>
       </c>
       <c r="E3" s="5">
-        <f>'Cost Data'!$B86</f>
+        <f>'Cost Data'!$B87</f>
         <v>2482.986689554888</v>
       </c>
       <c r="F3" s="5">
-        <f>'Cost Data'!$B86</f>
+        <f>'Cost Data'!$B87</f>
         <v>2482.986689554888</v>
       </c>
       <c r="G3" s="5">
-        <f>'Cost Data'!$B86</f>
+        <f>'Cost Data'!$B87</f>
         <v>2482.986689554888</v>
       </c>
       <c r="H3" s="5">
-        <f>'Cost Data'!$C86</f>
+        <f>'Cost Data'!$C87</f>
         <v>1950.9181132216977</v>
       </c>
     </row>
@@ -3149,23 +3219,23 @@
         <v>0</v>
       </c>
       <c r="C4" s="5">
-        <f>'Cost Data'!$B87</f>
+        <f>'Cost Data'!$B88</f>
         <v>2279318.9754813975</v>
       </c>
       <c r="D4" s="5">
-        <f>'Cost Data'!$B87</f>
+        <f>'Cost Data'!$B88</f>
         <v>2279318.9754813975</v>
       </c>
       <c r="E4" s="5">
-        <f>'Cost Data'!$B87</f>
+        <f>'Cost Data'!$B88</f>
         <v>2279318.9754813975</v>
       </c>
       <c r="F4" s="5">
-        <f>'Cost Data'!$B87</f>
+        <f>'Cost Data'!$B88</f>
         <v>2279318.9754813975</v>
       </c>
       <c r="G4" s="5">
-        <f>'Cost Data'!$B87</f>
+        <f>'Cost Data'!$B88</f>
         <v>2279318.9754813975</v>
       </c>
       <c r="H4" s="26">
@@ -3177,31 +3247,31 @@
         <v>5</v>
       </c>
       <c r="B5" s="5">
-        <f>'Cost Data'!$C88</f>
+        <f>'Cost Data'!$C89</f>
         <v>2434118.0622207024</v>
       </c>
       <c r="C5" s="5">
-        <f>'Cost Data'!$B88</f>
+        <f>'Cost Data'!$B89</f>
         <v>3332119.6733545554</v>
       </c>
       <c r="D5" s="5">
-        <f>'Cost Data'!$B88</f>
+        <f>'Cost Data'!$B89</f>
         <v>3332119.6733545554</v>
       </c>
       <c r="E5" s="5">
-        <f>'Cost Data'!$B88</f>
+        <f>'Cost Data'!$B89</f>
         <v>3332119.6733545554</v>
       </c>
       <c r="F5" s="5">
-        <f>'Cost Data'!$B88</f>
+        <f>'Cost Data'!$B89</f>
         <v>3332119.6733545554</v>
       </c>
       <c r="G5" s="5">
-        <f>'Cost Data'!$B88</f>
+        <f>'Cost Data'!$B89</f>
         <v>3332119.6733545554</v>
       </c>
       <c r="H5" s="5">
-        <f>'Cost Data'!$C88</f>
+        <f>'Cost Data'!$C89</f>
         <v>2434118.0622207024</v>
       </c>
     </row>
@@ -3213,23 +3283,23 @@
         <v>0</v>
       </c>
       <c r="C6" s="5">
-        <f>'Cost Data'!$B89</f>
+        <f>'Cost Data'!$B90</f>
         <v>3000</v>
       </c>
       <c r="D6" s="5">
-        <f>'Cost Data'!$B89</f>
+        <f>'Cost Data'!$B90</f>
         <v>3000</v>
       </c>
       <c r="E6" s="5">
-        <f>'Cost Data'!$B89</f>
+        <f>'Cost Data'!$B90</f>
         <v>3000</v>
       </c>
       <c r="F6" s="5">
-        <f>'Cost Data'!$B89</f>
+        <f>'Cost Data'!$B90</f>
         <v>3000</v>
       </c>
       <c r="G6" s="5">
-        <f>'Cost Data'!$B89</f>
+        <f>'Cost Data'!$B90</f>
         <v>3000</v>
       </c>
       <c r="H6" s="26">
@@ -3241,31 +3311,31 @@
         <v>7</v>
       </c>
       <c r="B7" s="5">
-        <f>'Cost Data'!$C90</f>
+        <f>'Cost Data'!$C91</f>
         <v>480.24283381885334</v>
       </c>
       <c r="C7" s="5">
-        <f>'Cost Data'!$B90</f>
+        <f>'Cost Data'!$B91</f>
         <v>914.32735845675347</v>
       </c>
       <c r="D7" s="5">
-        <f>'Cost Data'!$B90</f>
+        <f>'Cost Data'!$B91</f>
         <v>914.32735845675347</v>
       </c>
       <c r="E7" s="5">
-        <f>'Cost Data'!$B90</f>
+        <f>'Cost Data'!$B91</f>
         <v>914.32735845675347</v>
       </c>
       <c r="F7" s="5">
-        <f>'Cost Data'!$B90</f>
+        <f>'Cost Data'!$B91</f>
         <v>914.32735845675347</v>
       </c>
       <c r="G7" s="5">
-        <f>'Cost Data'!$B90</f>
+        <f>'Cost Data'!$B91</f>
         <v>914.32735845675347</v>
       </c>
       <c r="H7" s="5">
-        <f>'Cost Data'!$C90</f>
+        <f>'Cost Data'!$C91</f>
         <v>480.24283381885334</v>
       </c>
     </row>
@@ -3294,7 +3364,9 @@
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="A1:H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3337,31 +3409,31 @@
         <v>2</v>
       </c>
       <c r="B2" s="6">
-        <f>'Cost Data'!$C94</f>
+        <f>'Cost Data'!$C95</f>
         <v>344.72326776048766</v>
       </c>
       <c r="C2" s="6">
-        <f>'Cost Data'!$B94</f>
+        <f>'Cost Data'!$B95</f>
         <v>656.31362430473212</v>
       </c>
       <c r="D2" s="6">
-        <f>'Cost Data'!$B94</f>
+        <f>'Cost Data'!$B95</f>
         <v>656.31362430473212</v>
       </c>
       <c r="E2" s="6">
-        <f>'Cost Data'!$B94</f>
+        <f>'Cost Data'!$B95</f>
         <v>656.31362430473212</v>
       </c>
       <c r="F2" s="6">
-        <f>'Cost Data'!$B94</f>
+        <f>'Cost Data'!$B95</f>
         <v>656.31362430473212</v>
       </c>
       <c r="G2" s="6">
-        <f>'Cost Data'!$B94</f>
+        <f>'Cost Data'!$B95</f>
         <v>656.31362430473212</v>
       </c>
       <c r="H2" s="6">
-        <f>'Cost Data'!$C94</f>
+        <f>'Cost Data'!$C95</f>
         <v>344.72326776048766</v>
       </c>
     </row>
@@ -3370,31 +3442,31 @@
         <v>3</v>
       </c>
       <c r="B3" s="6">
-        <f>'Cost Data'!$C95</f>
-        <v>11785.714285714286</v>
+        <f>'Cost Data'!B25</f>
+        <v>17878.571428571428</v>
       </c>
       <c r="C3" s="6">
-        <f>'Cost Data'!$B95</f>
+        <f>'Cost Data'!$B96</f>
         <v>15000</v>
       </c>
       <c r="D3" s="6">
-        <f>'Cost Data'!$B95</f>
+        <f>'Cost Data'!$B96</f>
         <v>15000</v>
       </c>
       <c r="E3" s="6">
-        <f>'Cost Data'!$B95</f>
+        <f>'Cost Data'!$B96</f>
         <v>15000</v>
       </c>
       <c r="F3" s="6">
-        <f>'Cost Data'!$B95</f>
+        <f>'Cost Data'!$B96</f>
         <v>15000</v>
       </c>
       <c r="G3" s="6">
-        <f>'Cost Data'!$B95</f>
+        <f>'Cost Data'!$B96</f>
         <v>15000</v>
       </c>
       <c r="H3" s="6">
-        <f>'Cost Data'!$C95</f>
+        <f>'Cost Data'!$C96</f>
         <v>11785.714285714286</v>
       </c>
     </row>
@@ -3406,23 +3478,23 @@
         <v>0</v>
       </c>
       <c r="C4" s="6">
-        <f>'Cost Data'!$B96</f>
+        <f>'Cost Data'!$B97</f>
         <v>2279318.9754813975</v>
       </c>
       <c r="D4" s="6">
-        <f>'Cost Data'!$B96</f>
+        <f>'Cost Data'!$B97</f>
         <v>2279318.9754813975</v>
       </c>
       <c r="E4" s="6">
-        <f>'Cost Data'!$B96</f>
+        <f>'Cost Data'!$B97</f>
         <v>2279318.9754813975</v>
       </c>
       <c r="F4" s="6">
-        <f>'Cost Data'!$B96</f>
+        <f>'Cost Data'!$B97</f>
         <v>2279318.9754813975</v>
       </c>
       <c r="G4" s="6">
-        <f>'Cost Data'!$B96</f>
+        <f>'Cost Data'!$B97</f>
         <v>2279318.9754813975</v>
       </c>
       <c r="H4" s="26">
@@ -3434,31 +3506,31 @@
         <v>5</v>
       </c>
       <c r="B5" s="6">
-        <f>'Cost Data'!$C97</f>
+        <f>'Cost Data'!$C98</f>
         <v>2434118.0622207024</v>
       </c>
       <c r="C5" s="6">
-        <f>'Cost Data'!$B97</f>
+        <f>'Cost Data'!$B98</f>
         <v>3332119.6733545554</v>
       </c>
       <c r="D5" s="6">
-        <f>'Cost Data'!$B97</f>
+        <f>'Cost Data'!$B98</f>
         <v>3332119.6733545554</v>
       </c>
       <c r="E5" s="6">
-        <f>'Cost Data'!$B97</f>
+        <f>'Cost Data'!$B98</f>
         <v>3332119.6733545554</v>
       </c>
       <c r="F5" s="6">
-        <f>'Cost Data'!$B97</f>
+        <f>'Cost Data'!$B98</f>
         <v>3332119.6733545554</v>
       </c>
       <c r="G5" s="6">
-        <f>'Cost Data'!$B97</f>
+        <f>'Cost Data'!$B98</f>
         <v>3332119.6733545554</v>
       </c>
       <c r="H5" s="6">
-        <f>'Cost Data'!$C97</f>
+        <f>'Cost Data'!$C98</f>
         <v>2434118.0622207024</v>
       </c>
     </row>
@@ -3470,23 +3542,23 @@
         <v>0</v>
       </c>
       <c r="C6" s="6">
-        <f>'Cost Data'!$B98</f>
+        <f>'Cost Data'!$B99</f>
         <v>1695890</v>
       </c>
       <c r="D6" s="6">
-        <f>'Cost Data'!$B98</f>
+        <f>'Cost Data'!$B99</f>
         <v>1695890</v>
       </c>
       <c r="E6" s="6">
-        <f>'Cost Data'!$B98</f>
+        <f>'Cost Data'!$B99</f>
         <v>1695890</v>
       </c>
       <c r="F6" s="6">
-        <f>'Cost Data'!$B98</f>
+        <f>'Cost Data'!$B99</f>
         <v>1695890</v>
       </c>
       <c r="G6" s="6">
-        <f>'Cost Data'!$B98</f>
+        <f>'Cost Data'!$B99</f>
         <v>1695890</v>
       </c>
       <c r="H6" s="26">

</xml_diff>